<commit_message>
NEW-SRS: Ny indata för modeller och åtgärder
</commit_message>
<xml_diff>
--- a/src/main/resources/SRS_PM_indata_2_1.xlsx
+++ b/src/main/resources/SRS_PM_indata_2_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andersferrari/Dropbox/SKL/SRS/dokument/Åtgärder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8241A227-D0B5-4D40-9BD0-47C2E20BD69E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8634228B-ABF3-8E46-B4A4-9CD2D2EEBD44}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8840" yWindow="3560" windowWidth="18400" windowHeight="23340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5200" yWindow="460" windowWidth="18400" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kodning av variabelnamn" sheetId="1" r:id="rId1"/>
@@ -726,9 +726,6 @@
     <t>100%</t>
   </si>
   <si>
-    <t>Yrkesarbetar/Föräldraledig/Studerar</t>
-  </si>
-  <si>
     <t>not_unemp</t>
   </si>
   <si>
@@ -832,6 +829,9 @@
   </si>
   <si>
     <t>Haft annat sjukskrivningsfall som blev längre än 14 dagar i sträck, senaste 12 månaderna</t>
+  </si>
+  <si>
+    <t>Yrkesarbetar /Föräldraledig /Studerar</t>
   </si>
 </sst>
 </file>
@@ -1176,8 +1176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1204,10 +1204,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>262</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1218,7 +1218,7 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1964,7 +1964,7 @@
         <v>5</v>
       </c>
       <c r="D48" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F48" t="s">
         <v>177</v>
@@ -1978,7 +1978,7 @@
         <v>179</v>
       </c>
       <c r="E49" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -2017,7 +2017,7 @@
         <v>5</v>
       </c>
       <c r="E52" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -2058,8 +2058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2082,7 +2082,7 @@
         <v>195</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>196</v>
@@ -3693,16 +3693,16 @@
         <v>176</v>
       </c>
       <c r="B97" t="s">
-        <v>267</v>
+        <v>203</v>
       </c>
       <c r="C97" t="s">
-        <v>223</v>
+        <v>204</v>
       </c>
       <c r="D97">
         <v>1</v>
       </c>
       <c r="E97" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
@@ -3710,10 +3710,10 @@
         <v>176</v>
       </c>
       <c r="B98" t="s">
-        <v>225</v>
+        <v>266</v>
       </c>
       <c r="C98" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D98">
         <v>2</v>
@@ -3727,10 +3727,10 @@
         <v>176</v>
       </c>
       <c r="B99" t="s">
-        <v>268</v>
+        <v>225</v>
       </c>
       <c r="C99" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="D99">
         <v>3</v>
@@ -3744,16 +3744,16 @@
         <v>176</v>
       </c>
       <c r="B100" t="s">
-        <v>203</v>
+        <v>267</v>
       </c>
       <c r="C100" t="s">
-        <v>204</v>
+        <v>224</v>
       </c>
       <c r="D100">
         <v>4</v>
       </c>
       <c r="E100" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
@@ -3829,10 +3829,10 @@
         <v>183</v>
       </c>
       <c r="B105" t="s">
+        <v>235</v>
+      </c>
+      <c r="C105" t="s">
         <v>236</v>
-      </c>
-      <c r="C105" t="s">
-        <v>237</v>
       </c>
       <c r="D105">
         <v>1</v>
@@ -3846,10 +3846,10 @@
         <v>183</v>
       </c>
       <c r="B106" t="s">
+        <v>269</v>
+      </c>
+      <c r="C106" t="s">
         <v>234</v>
-      </c>
-      <c r="C106" t="s">
-        <v>235</v>
       </c>
       <c r="D106">
         <v>2</v>
@@ -3866,7 +3866,7 @@
         <v>197</v>
       </c>
       <c r="C107" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
@@ -3877,7 +3877,7 @@
         <v>197</v>
       </c>
       <c r="C108" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
@@ -3888,7 +3888,7 @@
         <v>206</v>
       </c>
       <c r="C109" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D109">
         <v>1</v>
@@ -3905,7 +3905,7 @@
         <v>203</v>
       </c>
       <c r="C110" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D110">
         <v>2</v>
@@ -3922,7 +3922,7 @@
         <v>206</v>
       </c>
       <c r="C111" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D111">
         <v>1</v>
@@ -3939,7 +3939,7 @@
         <v>203</v>
       </c>
       <c r="C112" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D112">
         <v>2</v>
@@ -3958,8 +3958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C208"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3969,18 +3969,18 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B2" t="s">
         <v>176</v>
@@ -3991,7 +3991,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B3" t="s">
         <v>183</v>
@@ -4002,7 +4002,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B4" t="s">
         <v>180</v>
@@ -4013,7 +4013,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B5" t="s">
         <v>164</v>
@@ -4024,7 +4024,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
@@ -4035,7 +4035,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -4046,7 +4046,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B8" t="s">
         <v>178</v>
@@ -4054,7 +4054,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B9" t="s">
         <v>186</v>
@@ -4062,7 +4062,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
@@ -4070,7 +4070,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B11" t="s">
         <v>176</v>
@@ -4081,7 +4081,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B12" t="s">
         <v>183</v>
@@ -4092,7 +4092,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B13" t="s">
         <v>180</v>
@@ -4103,7 +4103,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -4114,7 +4114,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B15" t="s">
         <v>98</v>
@@ -4125,7 +4125,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B16" t="s">
         <v>158</v>
@@ -4136,7 +4136,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B17" t="s">
         <v>178</v>
@@ -4144,7 +4144,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B18" t="s">
         <v>186</v>
@@ -4152,7 +4152,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B19" t="s">
         <v>4</v>
@@ -4160,7 +4160,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B20" t="s">
         <v>176</v>
@@ -4171,7 +4171,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B21" t="s">
         <v>183</v>
@@ -4182,7 +4182,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B22" t="s">
         <v>180</v>
@@ -4193,7 +4193,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B23" t="s">
         <v>101</v>
@@ -4204,7 +4204,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B24" t="s">
         <v>164</v>
@@ -4215,7 +4215,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B25" t="s">
         <v>18</v>
@@ -4226,7 +4226,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B26" t="s">
         <v>178</v>
@@ -4234,7 +4234,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B27" t="s">
         <v>186</v>
@@ -4242,7 +4242,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B28" t="s">
         <v>4</v>
@@ -4250,7 +4250,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B29" t="s">
         <v>176</v>
@@ -4261,7 +4261,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B30" t="s">
         <v>183</v>
@@ -4272,7 +4272,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B31" t="s">
         <v>180</v>
@@ -4283,7 +4283,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B32" t="s">
         <v>187</v>
@@ -4294,7 +4294,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B33" t="s">
         <v>104</v>
@@ -4305,7 +4305,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B34" t="s">
         <v>26</v>
@@ -4316,7 +4316,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B35" t="s">
         <v>178</v>
@@ -4324,7 +4324,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B36" t="s">
         <v>186</v>
@@ -4332,7 +4332,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B37" t="s">
         <v>4</v>
@@ -4430,7 +4430,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B47" t="s">
         <v>170</v>
@@ -4441,7 +4441,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B48" t="s">
         <v>176</v>
@@ -4452,7 +4452,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B49" t="s">
         <v>158</v>
@@ -4463,7 +4463,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B50" t="s">
         <v>180</v>
@@ -4474,7 +4474,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B51" t="s">
         <v>167</v>
@@ -4485,7 +4485,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B52" t="s">
         <v>107</v>
@@ -4496,7 +4496,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B53" t="s">
         <v>178</v>
@@ -4504,7 +4504,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B54" t="s">
         <v>186</v>
@@ -4512,7 +4512,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B55" t="s">
         <v>4</v>
@@ -4520,7 +4520,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B56" t="s">
         <v>176</v>
@@ -4531,7 +4531,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B57" t="s">
         <v>164</v>
@@ -4542,7 +4542,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B58" t="s">
         <v>30</v>
@@ -4553,7 +4553,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B59" t="s">
         <v>180</v>
@@ -4564,7 +4564,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B60" t="s">
         <v>90</v>
@@ -4575,7 +4575,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B61" t="s">
         <v>155</v>
@@ -4586,7 +4586,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B62" t="s">
         <v>178</v>
@@ -4594,7 +4594,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B63" t="s">
         <v>186</v>
@@ -4602,7 +4602,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B64" t="s">
         <v>4</v>
@@ -4610,7 +4610,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B65" t="s">
         <v>170</v>
@@ -4621,7 +4621,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B66" t="s">
         <v>167</v>
@@ -4632,7 +4632,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B67" t="s">
         <v>176</v>
@@ -4643,7 +4643,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B68" t="s">
         <v>180</v>
@@ -4654,7 +4654,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B69" t="s">
         <v>66</v>
@@ -4665,7 +4665,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B70" t="s">
         <v>187</v>
@@ -4676,7 +4676,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B71" t="s">
         <v>178</v>
@@ -4684,7 +4684,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B72" t="s">
         <v>186</v>
@@ -4692,7 +4692,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B73" t="s">
         <v>4</v>
@@ -4700,7 +4700,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B74" t="s">
         <v>170</v>
@@ -4711,7 +4711,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B75" t="s">
         <v>176</v>
@@ -4722,7 +4722,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B76" t="s">
         <v>50</v>
@@ -4733,7 +4733,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B77" t="s">
         <v>167</v>
@@ -4744,7 +4744,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B78" t="s">
         <v>46</v>
@@ -4755,7 +4755,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B79" t="s">
         <v>183</v>
@@ -4766,7 +4766,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B80" t="s">
         <v>178</v>
@@ -4774,7 +4774,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B81" t="s">
         <v>186</v>
@@ -4782,7 +4782,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B82" t="s">
         <v>4</v>
@@ -4790,7 +4790,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B83" t="s">
         <v>176</v>
@@ -4801,7 +4801,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B84" t="s">
         <v>170</v>
@@ -4812,7 +4812,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B85" t="s">
         <v>78</v>
@@ -4823,7 +4823,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B86" t="s">
         <v>183</v>
@@ -4834,7 +4834,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B87" t="s">
         <v>62</v>
@@ -4845,7 +4845,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B88" t="s">
         <v>167</v>
@@ -4856,7 +4856,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B89" t="s">
         <v>178</v>
@@ -4864,7 +4864,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B90" t="s">
         <v>186</v>
@@ -4872,7 +4872,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B91" t="s">
         <v>4</v>
@@ -4880,7 +4880,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B92" t="s">
         <v>170</v>
@@ -4891,7 +4891,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B93" t="s">
         <v>54</v>
@@ -4902,7 +4902,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B94" t="s">
         <v>50</v>
@@ -4913,7 +4913,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B95" t="s">
         <v>176</v>
@@ -4924,7 +4924,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B96" t="s">
         <v>158</v>
@@ -4935,7 +4935,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B97" t="s">
         <v>167</v>
@@ -4946,7 +4946,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B98" t="s">
         <v>178</v>
@@ -4954,7 +4954,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B99" t="s">
         <v>186</v>
@@ -4962,7 +4962,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B100" t="s">
         <v>4</v>
@@ -4970,7 +4970,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B101" t="s">
         <v>176</v>
@@ -4981,7 +4981,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B102" t="s">
         <v>170</v>
@@ -4992,7 +4992,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B103" t="s">
         <v>183</v>
@@ -5003,7 +5003,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B104" t="s">
         <v>180</v>
@@ -5014,7 +5014,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B105" t="s">
         <v>58</v>
@@ -5025,7 +5025,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B106" t="s">
         <v>107</v>
@@ -5036,7 +5036,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B107" t="s">
         <v>178</v>
@@ -5044,7 +5044,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B108" t="s">
         <v>186</v>
@@ -5052,7 +5052,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B109" t="s">
         <v>4</v>
@@ -5330,7 +5330,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B137" t="s">
         <v>176</v>
@@ -5341,7 +5341,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B138" t="s">
         <v>180</v>
@@ -5352,7 +5352,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B139" t="s">
         <v>170</v>
@@ -5363,7 +5363,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B140" t="s">
         <v>173</v>
@@ -5374,7 +5374,7 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B141" t="s">
         <v>86</v>
@@ -5385,7 +5385,7 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B142" t="s">
         <v>167</v>
@@ -5396,7 +5396,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B143" t="s">
         <v>178</v>
@@ -5404,7 +5404,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B144" t="s">
         <v>186</v>
@@ -5412,7 +5412,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B145" t="s">
         <v>4</v>
@@ -5420,7 +5420,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B146" t="s">
         <v>176</v>
@@ -5431,7 +5431,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B147" t="s">
         <v>94</v>
@@ -5442,7 +5442,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B148" t="s">
         <v>183</v>
@@ -5453,7 +5453,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B149" t="s">
         <v>180</v>
@@ -5464,7 +5464,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B150" t="s">
         <v>161</v>
@@ -5475,7 +5475,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B151" t="s">
         <v>78</v>
@@ -5486,7 +5486,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B152" t="s">
         <v>178</v>
@@ -5494,7 +5494,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B153" t="s">
         <v>186</v>
@@ -5502,7 +5502,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B154" t="s">
         <v>4</v>
@@ -5600,7 +5600,7 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B164" t="s">
         <v>176</v>
@@ -5611,7 +5611,7 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B165" t="s">
         <v>180</v>
@@ -5622,7 +5622,7 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B166" t="s">
         <v>119</v>
@@ -5633,7 +5633,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B167" t="s">
         <v>42</v>
@@ -5644,7 +5644,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B168" t="s">
         <v>164</v>
@@ -5655,7 +5655,7 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B169" t="s">
         <v>155</v>
@@ -5666,7 +5666,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B170" t="s">
         <v>178</v>
@@ -5674,7 +5674,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B171" t="s">
         <v>186</v>
@@ -5682,7 +5682,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B172" t="s">
         <v>4</v>
@@ -5690,7 +5690,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B173" t="s">
         <v>176</v>
@@ -5701,7 +5701,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B174" t="s">
         <v>180</v>
@@ -5712,7 +5712,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B175" t="s">
         <v>167</v>
@@ -5723,7 +5723,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B176" t="s">
         <v>158</v>
@@ -5734,7 +5734,7 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B177" t="s">
         <v>123</v>
@@ -5745,7 +5745,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B178" t="s">
         <v>170</v>
@@ -5756,7 +5756,7 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B179" t="s">
         <v>178</v>
@@ -5764,7 +5764,7 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B180" t="s">
         <v>186</v>
@@ -5772,7 +5772,7 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B181" t="s">
         <v>4</v>
@@ -5780,7 +5780,7 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B182" t="s">
         <v>127</v>
@@ -5791,7 +5791,7 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B183" t="s">
         <v>176</v>
@@ -5802,7 +5802,7 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B184" t="s">
         <v>131</v>
@@ -5813,7 +5813,7 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B185" t="s">
         <v>135</v>
@@ -5824,7 +5824,7 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B186" t="s">
         <v>190</v>
@@ -5835,7 +5835,7 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B187" t="s">
         <v>180</v>
@@ -5846,7 +5846,7 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B188" t="s">
         <v>178</v>
@@ -5854,7 +5854,7 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B189" t="s">
         <v>186</v>
@@ -5862,7 +5862,7 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B190" t="s">
         <v>4</v>
@@ -5870,7 +5870,7 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B191" t="s">
         <v>147</v>
@@ -5881,7 +5881,7 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B192" t="s">
         <v>167</v>
@@ -5892,7 +5892,7 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B193" t="s">
         <v>143</v>
@@ -5903,7 +5903,7 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B194" t="s">
         <v>158</v>
@@ -5914,7 +5914,7 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B195" t="s">
         <v>176</v>
@@ -5925,7 +5925,7 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B196" t="s">
         <v>139</v>
@@ -5936,7 +5936,7 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B197" t="s">
         <v>178</v>
@@ -5944,7 +5944,7 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B198" t="s">
         <v>186</v>
@@ -5952,7 +5952,7 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B199" t="s">
         <v>4</v>
@@ -5960,7 +5960,7 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B200" t="s">
         <v>176</v>
@@ -5971,7 +5971,7 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B201" t="s">
         <v>167</v>
@@ -5982,7 +5982,7 @@
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B202" t="s">
         <v>158</v>
@@ -5993,7 +5993,7 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B203" t="s">
         <v>151</v>
@@ -6004,7 +6004,7 @@
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B204" t="s">
         <v>90</v>
@@ -6015,7 +6015,7 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B205" t="s">
         <v>180</v>
@@ -6026,7 +6026,7 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B206" t="s">
         <v>178</v>
@@ -6034,7 +6034,7 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B207" t="s">
         <v>186</v>
@@ -6042,7 +6042,7 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B208" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
NEW-SRS: New indata (questions and answers) for prediction models, also updated filter to skip non factor variables.
</commit_message>
<xml_diff>
--- a/src/main/resources/SRS_PM_indata_2_1.xlsx
+++ b/src/main/resources/SRS_PM_indata_2_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andersferrari/Dropbox/SKL/SRS/dokument/Åtgärder/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andersferrari/Dropbox/SKL/SRS/Indata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8634228B-ABF3-8E46-B4A4-9CD2D2EEBD44}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{95A6247C-28F1-AA44-AABB-10CA8ED7EC73}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5200" yWindow="460" windowWidth="18400" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38340" windowHeight="22420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kodning av variabelnamn" sheetId="1" r:id="rId1"/>
@@ -831,7 +831,7 @@
     <t>Haft annat sjukskrivningsfall som blev längre än 14 dagar i sträck, senaste 12 månaderna</t>
   </si>
   <si>
-    <t>Yrkesarbetar /Föräldraledig /Studerar</t>
+    <t>Yrkesarbetar, Föräldraledig, Studerar</t>
   </si>
 </sst>
 </file>
@@ -875,9 +875,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1176,7 +1177,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
@@ -2058,8 +2059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E112"/>
   <sheetViews>
-    <sheetView topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="D97" sqref="D97"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F102" sqref="F102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3958,8 +3959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C208"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3979,2074 +3980,2143 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>178</v>
       </c>
+      <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>186</v>
       </c>
+      <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>178</v>
       </c>
+      <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>186</v>
       </c>
+      <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="A22" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="A23" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="A24" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="A25" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="A26" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="2" t="s">
         <v>178</v>
       </c>
+      <c r="C26" s="2"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="A27" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="2" t="s">
         <v>186</v>
       </c>
+      <c r="C27" s="2"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="A28" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="A29" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="A30" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="A31" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="A32" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="A33" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="A34" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="A35" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2" t="s">
         <v>178</v>
       </c>
+      <c r="C35" s="2"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="A36" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="2" t="s">
         <v>186</v>
       </c>
+      <c r="C36" s="2"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="A37" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C37" s="2"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="A38" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="A39" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="A40" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="A41" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="A42" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="A43" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="A44" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="2" t="s">
         <v>178</v>
       </c>
+      <c r="C44" s="2"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="A45" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="2" t="s">
         <v>186</v>
       </c>
+      <c r="C45" s="2"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="A46" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C46" s="2"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="A47" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+      <c r="A48" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C48" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C48">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="C49" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C50" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C51" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C52" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C53" s="2"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C54" s="2"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55" s="2"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C56" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C57" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C58" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C59" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C60" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C61" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C62" s="2"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C63" s="2"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C64" s="2"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C65" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C66" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C67" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C68" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C69" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C70" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C71" s="2"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C72" s="2"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C73" s="2"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C74" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C75" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C76" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C77" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C78" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C49">
+      <c r="C79" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C80" s="2"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C81" s="2"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C82" s="2"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C83" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C84" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C85" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>247</v>
-      </c>
-      <c r="B50" t="s">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C86" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C87" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C88" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C89" s="2"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C90" s="2"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C91" s="2"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C92" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C93" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C94" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C95" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C96" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C97" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C98" s="2"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C99" s="2"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C100" s="2"/>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C101" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C102" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C103" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B104" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C50">
+      <c r="C104" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>247</v>
-      </c>
-      <c r="B51" t="s">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C105" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C106" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C107" s="2"/>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C108" s="2"/>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C109" s="2"/>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C110" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C111" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C112" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C113" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C114" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B115" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C51">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>247</v>
-      </c>
-      <c r="B52" t="s">
-        <v>107</v>
-      </c>
-      <c r="C52">
+      <c r="C115" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>247</v>
-      </c>
-      <c r="B53" t="s">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B116" s="2" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>247</v>
-      </c>
-      <c r="B54" t="s">
+      <c r="C116" s="2"/>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A117" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B117" s="2" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>247</v>
-      </c>
-      <c r="B55" t="s">
+      <c r="C117" s="2"/>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B118" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>248</v>
-      </c>
-      <c r="B56" t="s">
+      <c r="C118" s="2"/>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B119" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>248</v>
-      </c>
-      <c r="B57" t="s">
+      <c r="C119" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C120" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C121" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C122" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C123" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C124" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C125" s="2"/>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C126" s="2"/>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C127" s="2"/>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C128" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C129" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C130" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C131" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A132" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C132" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C133" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C134" s="2"/>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C135" s="2"/>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C136" s="2"/>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C137" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A138" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C138" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A139" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C139" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A140" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C140" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A141" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C141" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A142" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C142" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A143" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C143" s="2"/>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A144" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C144" s="2"/>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A145" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C145" s="2"/>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A146" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C146" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A147" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C147" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A148" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C148" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A149" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C149" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A150" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C150" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A151" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C151" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A152" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C152" s="2"/>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A153" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C153" s="2"/>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A154" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C154" s="2"/>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A155" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C155" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A156" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C156" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A157" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C157" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A158" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C158" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A159" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C159" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A160" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C160" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A161" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C161" s="2"/>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A162" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C162" s="2"/>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A163" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C163" s="2"/>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A164" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C164" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A165" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C165" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A166" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C166" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A167" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C167" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A168" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C168" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A169" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B169" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C57">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>248</v>
-      </c>
-      <c r="B58" t="s">
-        <v>30</v>
-      </c>
-      <c r="C58">
+      <c r="C169" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A170" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C170" s="2"/>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A171" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C171" s="2"/>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A172" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C172" s="2"/>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A173" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C173" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A174" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C174" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A175" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C175" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>248</v>
-      </c>
-      <c r="B59" t="s">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A176" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C176" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A177" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C177" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A178" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C178" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A179" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C179" s="2"/>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A180" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C180" s="2"/>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A181" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C181" s="2"/>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A182" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C182" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A183" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C183" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A184" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C184" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A185" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C185" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A186" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C186" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A187" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B187" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C59">
+      <c r="C187" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A188" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C188" s="2"/>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A189" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C189" s="2"/>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A190" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B190" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>248</v>
-      </c>
-      <c r="B60" t="s">
+      <c r="C190" s="2"/>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A191" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C191" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A192" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C192" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A193" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C193" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A194" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C194" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A195" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C195" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A196" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C196" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A197" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C197" s="2"/>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A198" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C198" s="2"/>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A199" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C199" s="2"/>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A200" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B200" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C200" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A201" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B201" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C201" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A202" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B202" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C202" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A203" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C203" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A204" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B204" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C60">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>248</v>
-      </c>
-      <c r="B61" t="s">
-        <v>155</v>
-      </c>
-      <c r="C61">
+      <c r="C204" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A205" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B205" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C205" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>248</v>
-      </c>
-      <c r="B62" t="s">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A206" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B206" s="2" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>248</v>
-      </c>
-      <c r="B63" t="s">
+      <c r="C206" s="2"/>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A207" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B207" s="2" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>248</v>
-      </c>
-      <c r="B64" t="s">
+      <c r="C207" s="2"/>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A208" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B208" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>249</v>
-      </c>
-      <c r="B65" t="s">
-        <v>170</v>
-      </c>
-      <c r="C65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>249</v>
-      </c>
-      <c r="B66" t="s">
-        <v>167</v>
-      </c>
-      <c r="C66">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>249</v>
-      </c>
-      <c r="B67" t="s">
-        <v>176</v>
-      </c>
-      <c r="C67">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>249</v>
-      </c>
-      <c r="B68" t="s">
-        <v>180</v>
-      </c>
-      <c r="C68">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>249</v>
-      </c>
-      <c r="B69" t="s">
-        <v>66</v>
-      </c>
-      <c r="C69">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>249</v>
-      </c>
-      <c r="B70" t="s">
-        <v>187</v>
-      </c>
-      <c r="C70">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>249</v>
-      </c>
-      <c r="B71" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>249</v>
-      </c>
-      <c r="B72" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>249</v>
-      </c>
-      <c r="B73" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>250</v>
-      </c>
-      <c r="B74" t="s">
-        <v>170</v>
-      </c>
-      <c r="C74">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>250</v>
-      </c>
-      <c r="B75" t="s">
-        <v>176</v>
-      </c>
-      <c r="C75">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>250</v>
-      </c>
-      <c r="B76" t="s">
-        <v>50</v>
-      </c>
-      <c r="C76">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>250</v>
-      </c>
-      <c r="B77" t="s">
-        <v>167</v>
-      </c>
-      <c r="C77">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>250</v>
-      </c>
-      <c r="B78" t="s">
-        <v>46</v>
-      </c>
-      <c r="C78">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>250</v>
-      </c>
-      <c r="B79" t="s">
-        <v>183</v>
-      </c>
-      <c r="C79">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>250</v>
-      </c>
-      <c r="B80" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>250</v>
-      </c>
-      <c r="B81" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>250</v>
-      </c>
-      <c r="B82" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>251</v>
-      </c>
-      <c r="B83" t="s">
-        <v>176</v>
-      </c>
-      <c r="C83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>251</v>
-      </c>
-      <c r="B84" t="s">
-        <v>170</v>
-      </c>
-      <c r="C84">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>251</v>
-      </c>
-      <c r="B85" t="s">
-        <v>78</v>
-      </c>
-      <c r="C85">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>251</v>
-      </c>
-      <c r="B86" t="s">
-        <v>183</v>
-      </c>
-      <c r="C86">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>251</v>
-      </c>
-      <c r="B87" t="s">
-        <v>62</v>
-      </c>
-      <c r="C87">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>251</v>
-      </c>
-      <c r="B88" t="s">
-        <v>167</v>
-      </c>
-      <c r="C88">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
-        <v>251</v>
-      </c>
-      <c r="B89" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
-        <v>251</v>
-      </c>
-      <c r="B90" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
-        <v>251</v>
-      </c>
-      <c r="B91" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>252</v>
-      </c>
-      <c r="B92" t="s">
-        <v>170</v>
-      </c>
-      <c r="C92">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>252</v>
-      </c>
-      <c r="B93" t="s">
-        <v>54</v>
-      </c>
-      <c r="C93">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
-        <v>252</v>
-      </c>
-      <c r="B94" t="s">
-        <v>50</v>
-      </c>
-      <c r="C94">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
-        <v>252</v>
-      </c>
-      <c r="B95" t="s">
-        <v>176</v>
-      </c>
-      <c r="C95">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>252</v>
-      </c>
-      <c r="B96" t="s">
-        <v>158</v>
-      </c>
-      <c r="C96">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
-        <v>252</v>
-      </c>
-      <c r="B97" t="s">
-        <v>167</v>
-      </c>
-      <c r="C97">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
-        <v>252</v>
-      </c>
-      <c r="B98" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
-        <v>252</v>
-      </c>
-      <c r="B99" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
-        <v>252</v>
-      </c>
-      <c r="B100" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
-        <v>253</v>
-      </c>
-      <c r="B101" t="s">
-        <v>176</v>
-      </c>
-      <c r="C101">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
-        <v>253</v>
-      </c>
-      <c r="B102" t="s">
-        <v>170</v>
-      </c>
-      <c r="C102">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
-        <v>253</v>
-      </c>
-      <c r="B103" t="s">
-        <v>183</v>
-      </c>
-      <c r="C103">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
-        <v>253</v>
-      </c>
-      <c r="B104" t="s">
-        <v>180</v>
-      </c>
-      <c r="C104">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
-        <v>253</v>
-      </c>
-      <c r="B105" t="s">
-        <v>58</v>
-      </c>
-      <c r="C105">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
-        <v>253</v>
-      </c>
-      <c r="B106" t="s">
-        <v>107</v>
-      </c>
-      <c r="C106">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
-        <v>253</v>
-      </c>
-      <c r="B107" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
-        <v>253</v>
-      </c>
-      <c r="B108" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
-        <v>253</v>
-      </c>
-      <c r="B109" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
-        <v>63</v>
-      </c>
-      <c r="B110" t="s">
-        <v>176</v>
-      </c>
-      <c r="C110">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
-        <v>63</v>
-      </c>
-      <c r="B111" t="s">
-        <v>183</v>
-      </c>
-      <c r="C111">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A112" t="s">
-        <v>63</v>
-      </c>
-      <c r="B112" t="s">
-        <v>180</v>
-      </c>
-      <c r="C112">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
-        <v>63</v>
-      </c>
-      <c r="B113" t="s">
-        <v>22</v>
-      </c>
-      <c r="C113">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
-        <v>63</v>
-      </c>
-      <c r="B114" t="s">
-        <v>94</v>
-      </c>
-      <c r="C114">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
-        <v>63</v>
-      </c>
-      <c r="B115" t="s">
-        <v>167</v>
-      </c>
-      <c r="C115">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
-        <v>63</v>
-      </c>
-      <c r="B116" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
-        <v>63</v>
-      </c>
-      <c r="B117" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
-        <v>63</v>
-      </c>
-      <c r="B118" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
-        <v>67</v>
-      </c>
-      <c r="B119" t="s">
-        <v>176</v>
-      </c>
-      <c r="C119">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
-        <v>67</v>
-      </c>
-      <c r="B120" t="s">
-        <v>180</v>
-      </c>
-      <c r="C120">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A121" t="s">
-        <v>67</v>
-      </c>
-      <c r="B121" t="s">
-        <v>183</v>
-      </c>
-      <c r="C121">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A122" t="s">
-        <v>67</v>
-      </c>
-      <c r="B122" t="s">
-        <v>161</v>
-      </c>
-      <c r="C122">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A123" t="s">
-        <v>67</v>
-      </c>
-      <c r="B123" t="s">
-        <v>74</v>
-      </c>
-      <c r="C123">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A124" t="s">
-        <v>67</v>
-      </c>
-      <c r="B124" t="s">
-        <v>70</v>
-      </c>
-      <c r="C124">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A125" t="s">
-        <v>67</v>
-      </c>
-      <c r="B125" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A126" t="s">
-        <v>67</v>
-      </c>
-      <c r="B126" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A127" t="s">
-        <v>67</v>
-      </c>
-      <c r="B127" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A128" t="s">
-        <v>79</v>
-      </c>
-      <c r="B128" t="s">
-        <v>170</v>
-      </c>
-      <c r="C128">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
-        <v>79</v>
-      </c>
-      <c r="B129" t="s">
-        <v>176</v>
-      </c>
-      <c r="C129">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
-        <v>79</v>
-      </c>
-      <c r="B130" t="s">
-        <v>167</v>
-      </c>
-      <c r="C130">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
-        <v>79</v>
-      </c>
-      <c r="B131" t="s">
-        <v>158</v>
-      </c>
-      <c r="C131">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A132" t="s">
-        <v>79</v>
-      </c>
-      <c r="B132" t="s">
-        <v>180</v>
-      </c>
-      <c r="C132">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A133" t="s">
-        <v>79</v>
-      </c>
-      <c r="B133" t="s">
-        <v>82</v>
-      </c>
-      <c r="C133">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A134" t="s">
-        <v>79</v>
-      </c>
-      <c r="B134" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A135" t="s">
-        <v>79</v>
-      </c>
-      <c r="B135" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A136" t="s">
-        <v>79</v>
-      </c>
-      <c r="B136" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A137" t="s">
-        <v>254</v>
-      </c>
-      <c r="B137" t="s">
-        <v>176</v>
-      </c>
-      <c r="C137">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A138" t="s">
-        <v>254</v>
-      </c>
-      <c r="B138" t="s">
-        <v>180</v>
-      </c>
-      <c r="C138">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A139" t="s">
-        <v>254</v>
-      </c>
-      <c r="B139" t="s">
-        <v>170</v>
-      </c>
-      <c r="C139">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A140" t="s">
-        <v>254</v>
-      </c>
-      <c r="B140" t="s">
-        <v>173</v>
-      </c>
-      <c r="C140">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A141" t="s">
-        <v>254</v>
-      </c>
-      <c r="B141" t="s">
-        <v>86</v>
-      </c>
-      <c r="C141">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A142" t="s">
-        <v>254</v>
-      </c>
-      <c r="B142" t="s">
-        <v>167</v>
-      </c>
-      <c r="C142">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A143" t="s">
-        <v>254</v>
-      </c>
-      <c r="B143" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A144" t="s">
-        <v>254</v>
-      </c>
-      <c r="B144" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A145" t="s">
-        <v>254</v>
-      </c>
-      <c r="B145" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A146" t="s">
-        <v>255</v>
-      </c>
-      <c r="B146" t="s">
-        <v>176</v>
-      </c>
-      <c r="C146">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A147" t="s">
-        <v>255</v>
-      </c>
-      <c r="B147" t="s">
-        <v>94</v>
-      </c>
-      <c r="C147">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A148" t="s">
-        <v>255</v>
-      </c>
-      <c r="B148" t="s">
-        <v>183</v>
-      </c>
-      <c r="C148">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A149" t="s">
-        <v>255</v>
-      </c>
-      <c r="B149" t="s">
-        <v>180</v>
-      </c>
-      <c r="C149">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A150" t="s">
-        <v>255</v>
-      </c>
-      <c r="B150" t="s">
-        <v>161</v>
-      </c>
-      <c r="C150">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A151" t="s">
-        <v>255</v>
-      </c>
-      <c r="B151" t="s">
-        <v>78</v>
-      </c>
-      <c r="C151">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A152" t="s">
-        <v>255</v>
-      </c>
-      <c r="B152" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A153" t="s">
-        <v>255</v>
-      </c>
-      <c r="B153" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A154" t="s">
-        <v>255</v>
-      </c>
-      <c r="B154" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A155" t="s">
-        <v>108</v>
-      </c>
-      <c r="B155" t="s">
-        <v>176</v>
-      </c>
-      <c r="C155">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A156" t="s">
-        <v>108</v>
-      </c>
-      <c r="B156" t="s">
-        <v>183</v>
-      </c>
-      <c r="C156">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A157" t="s">
-        <v>108</v>
-      </c>
-      <c r="B157" t="s">
-        <v>180</v>
-      </c>
-      <c r="C157">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A158" t="s">
-        <v>108</v>
-      </c>
-      <c r="B158" t="s">
-        <v>115</v>
-      </c>
-      <c r="C158">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A159" t="s">
-        <v>108</v>
-      </c>
-      <c r="B159" t="s">
-        <v>111</v>
-      </c>
-      <c r="C159">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A160" t="s">
-        <v>108</v>
-      </c>
-      <c r="B160" t="s">
-        <v>173</v>
-      </c>
-      <c r="C160">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A161" t="s">
-        <v>108</v>
-      </c>
-      <c r="B161" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A162" t="s">
-        <v>108</v>
-      </c>
-      <c r="B162" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A163" t="s">
-        <v>108</v>
-      </c>
-      <c r="B163" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A164" t="s">
-        <v>256</v>
-      </c>
-      <c r="B164" t="s">
-        <v>176</v>
-      </c>
-      <c r="C164">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A165" t="s">
-        <v>256</v>
-      </c>
-      <c r="B165" t="s">
-        <v>180</v>
-      </c>
-      <c r="C165">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A166" t="s">
-        <v>256</v>
-      </c>
-      <c r="B166" t="s">
-        <v>119</v>
-      </c>
-      <c r="C166">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A167" t="s">
-        <v>256</v>
-      </c>
-      <c r="B167" t="s">
-        <v>42</v>
-      </c>
-      <c r="C167">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A168" t="s">
-        <v>256</v>
-      </c>
-      <c r="B168" t="s">
-        <v>164</v>
-      </c>
-      <c r="C168">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A169" t="s">
-        <v>256</v>
-      </c>
-      <c r="B169" t="s">
-        <v>155</v>
-      </c>
-      <c r="C169">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A170" t="s">
-        <v>256</v>
-      </c>
-      <c r="B170" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A171" t="s">
-        <v>256</v>
-      </c>
-      <c r="B171" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A172" t="s">
-        <v>256</v>
-      </c>
-      <c r="B172" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A173" t="s">
-        <v>257</v>
-      </c>
-      <c r="B173" t="s">
-        <v>176</v>
-      </c>
-      <c r="C173">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A174" t="s">
-        <v>257</v>
-      </c>
-      <c r="B174" t="s">
-        <v>180</v>
-      </c>
-      <c r="C174">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A175" t="s">
-        <v>257</v>
-      </c>
-      <c r="B175" t="s">
-        <v>167</v>
-      </c>
-      <c r="C175">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A176" t="s">
-        <v>257</v>
-      </c>
-      <c r="B176" t="s">
-        <v>158</v>
-      </c>
-      <c r="C176">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A177" t="s">
-        <v>257</v>
-      </c>
-      <c r="B177" t="s">
-        <v>123</v>
-      </c>
-      <c r="C177">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A178" t="s">
-        <v>257</v>
-      </c>
-      <c r="B178" t="s">
-        <v>170</v>
-      </c>
-      <c r="C178">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A179" t="s">
-        <v>257</v>
-      </c>
-      <c r="B179" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A180" t="s">
-        <v>257</v>
-      </c>
-      <c r="B180" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A181" t="s">
-        <v>257</v>
-      </c>
-      <c r="B181" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A182" t="s">
-        <v>258</v>
-      </c>
-      <c r="B182" t="s">
-        <v>127</v>
-      </c>
-      <c r="C182">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A183" t="s">
-        <v>258</v>
-      </c>
-      <c r="B183" t="s">
-        <v>176</v>
-      </c>
-      <c r="C183">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A184" t="s">
-        <v>258</v>
-      </c>
-      <c r="B184" t="s">
-        <v>131</v>
-      </c>
-      <c r="C184">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A185" t="s">
-        <v>258</v>
-      </c>
-      <c r="B185" t="s">
-        <v>135</v>
-      </c>
-      <c r="C185">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A186" t="s">
-        <v>258</v>
-      </c>
-      <c r="B186" t="s">
-        <v>190</v>
-      </c>
-      <c r="C186">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A187" t="s">
-        <v>258</v>
-      </c>
-      <c r="B187" t="s">
-        <v>180</v>
-      </c>
-      <c r="C187">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A188" t="s">
-        <v>258</v>
-      </c>
-      <c r="B188" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A189" t="s">
-        <v>258</v>
-      </c>
-      <c r="B189" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A190" t="s">
-        <v>258</v>
-      </c>
-      <c r="B190" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A191" t="s">
-        <v>259</v>
-      </c>
-      <c r="B191" t="s">
-        <v>147</v>
-      </c>
-      <c r="C191">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A192" t="s">
-        <v>259</v>
-      </c>
-      <c r="B192" t="s">
-        <v>167</v>
-      </c>
-      <c r="C192">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A193" t="s">
-        <v>259</v>
-      </c>
-      <c r="B193" t="s">
-        <v>143</v>
-      </c>
-      <c r="C193">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A194" t="s">
-        <v>259</v>
-      </c>
-      <c r="B194" t="s">
-        <v>158</v>
-      </c>
-      <c r="C194">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A195" t="s">
-        <v>259</v>
-      </c>
-      <c r="B195" t="s">
-        <v>176</v>
-      </c>
-      <c r="C195">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A196" t="s">
-        <v>259</v>
-      </c>
-      <c r="B196" t="s">
-        <v>139</v>
-      </c>
-      <c r="C196">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A197" t="s">
-        <v>259</v>
-      </c>
-      <c r="B197" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A198" t="s">
-        <v>259</v>
-      </c>
-      <c r="B198" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A199" t="s">
-        <v>259</v>
-      </c>
-      <c r="B199" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A200" t="s">
-        <v>260</v>
-      </c>
-      <c r="B200" t="s">
-        <v>176</v>
-      </c>
-      <c r="C200">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A201" t="s">
-        <v>260</v>
-      </c>
-      <c r="B201" t="s">
-        <v>167</v>
-      </c>
-      <c r="C201">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A202" t="s">
-        <v>260</v>
-      </c>
-      <c r="B202" t="s">
-        <v>158</v>
-      </c>
-      <c r="C202">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A203" t="s">
-        <v>260</v>
-      </c>
-      <c r="B203" t="s">
-        <v>151</v>
-      </c>
-      <c r="C203">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A204" t="s">
-        <v>260</v>
-      </c>
-      <c r="B204" t="s">
-        <v>90</v>
-      </c>
-      <c r="C204">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A205" t="s">
-        <v>260</v>
-      </c>
-      <c r="B205" t="s">
-        <v>180</v>
-      </c>
-      <c r="C205">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A206" t="s">
-        <v>260</v>
-      </c>
-      <c r="B206" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A207" t="s">
-        <v>260</v>
-      </c>
-      <c r="B207" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A208" t="s">
-        <v>260</v>
-      </c>
-      <c r="B208" t="s">
-        <v>4</v>
-      </c>
+      <c r="C208" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>